<commit_message>
Fix buffer PCA FTE display and popover positioning
- Fix buffer PCA showing incorrect FTE (0.5 -> 1.0) in Step 2.1 and Staff Pool
  - Remove slot clamp that excluded buffer PCA from Step 2.1 when missing slots didn't match
  - Fix BufferStaffPool true FTE calculation to use buffer_fte instead of availableSlots.length
  - Update Step 2.1 dialog to show buffer capacity correctly
- Change popovers from fixed to absolute positioning so they scroll with page
  - Update position calculation to store document coordinates (client + scrollX/Y)
  - Affects StaffContextMenu, TeamPickerPopover, ConfirmPopover, SlotSelectionPopover, and inline popovers
- Update journal.md with Phase 22
</commit_message>
<xml_diff>
--- a/12_2025 Manpower.xlsx
+++ b/12_2025 Manpower.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvin/Desktop/RBIP duty list web app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E1B4C8-B61F-3342-A809-EAF1034C439B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F7794B-A010-FD4D-B642-AE6CA74C1380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40960" yWindow="620" windowWidth="38400" windowHeight="20980" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40960" yWindow="620" windowWidth="38400" windowHeight="20980" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="8 Aug " sheetId="13" state="hidden" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4379" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4379" uniqueCount="487">
   <si>
     <t>Team</t>
   </si>
@@ -2484,6 +2484,29 @@
     <t>Harry Wed 0.25am + 0.25pm + neuro gym
 Fri 0.25pm + neuro gym</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Total no. of SS on duty = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="28"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">13 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="28"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> on Mon-Fri (Effective from 12/11/20), at least 1 SS per team over the whole day </t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -5443,6 +5466,15 @@
     <xf numFmtId="0" fontId="74" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="70" fillId="26" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="26" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="46" fillId="9" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5532,15 +5564,6 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="9" borderId="23" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="26" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="26" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -5986,12 +6009,12 @@
       <c r="O3" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="583" t="s">
+      <c r="P3" s="586" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="584"/>
-      <c r="R3" s="584"/>
-      <c r="S3" s="585"/>
+      <c r="Q3" s="587"/>
+      <c r="R3" s="587"/>
+      <c r="S3" s="588"/>
       <c r="T3" s="27" t="s">
         <v>18</v>
       </c>
@@ -6637,12 +6660,12 @@
       <c r="O17" s="142">
         <v>0.4</v>
       </c>
-      <c r="P17" s="586" t="s">
+      <c r="P17" s="589" t="s">
         <v>195</v>
       </c>
-      <c r="Q17" s="587"/>
-      <c r="R17" s="588"/>
-      <c r="S17" s="589"/>
+      <c r="Q17" s="590"/>
+      <c r="R17" s="591"/>
+      <c r="S17" s="592"/>
       <c r="T17" s="143" t="s">
         <v>88</v>
       </c>
@@ -6696,10 +6719,10 @@
         <f>N18+O17</f>
         <v>1.0428571428571427</v>
       </c>
-      <c r="P18" s="590"/>
-      <c r="Q18" s="591"/>
-      <c r="R18" s="591"/>
-      <c r="S18" s="592"/>
+      <c r="P18" s="593"/>
+      <c r="Q18" s="594"/>
+      <c r="R18" s="594"/>
+      <c r="S18" s="595"/>
       <c r="T18" s="153" t="s">
         <v>89</v>
       </c>
@@ -6729,12 +6752,12 @@
       <c r="M19" s="107"/>
       <c r="N19" s="56"/>
       <c r="O19" s="107"/>
-      <c r="P19" s="593" t="s">
+      <c r="P19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="Q19" s="594"/>
-      <c r="R19" s="594"/>
-      <c r="S19" s="595"/>
+      <c r="Q19" s="597"/>
+      <c r="R19" s="597"/>
+      <c r="S19" s="598"/>
       <c r="T19" s="161"/>
       <c r="U19" s="117"/>
       <c r="V19" s="162"/>
@@ -6768,10 +6791,10 @@
       <c r="M20" s="107"/>
       <c r="N20" s="24"/>
       <c r="O20" s="107"/>
-      <c r="P20" s="596"/>
-      <c r="Q20" s="597"/>
-      <c r="R20" s="597"/>
-      <c r="S20" s="598"/>
+      <c r="P20" s="599"/>
+      <c r="Q20" s="600"/>
+      <c r="R20" s="600"/>
+      <c r="S20" s="601"/>
       <c r="T20" s="161"/>
       <c r="U20" s="117"/>
       <c r="V20" s="162"/>
@@ -6831,11 +6854,11 @@
       <c r="N22" s="24"/>
       <c r="O22" s="20"/>
       <c r="P22" s="168"/>
-      <c r="Q22" s="599" t="s">
+      <c r="Q22" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="R22" s="599"/>
-      <c r="S22" s="600"/>
+      <c r="R22" s="602"/>
+      <c r="S22" s="603"/>
       <c r="T22" s="161"/>
       <c r="U22" s="117"/>
       <c r="V22" s="162"/>
@@ -6862,10 +6885,10 @@
       <c r="M23" s="175"/>
       <c r="N23" s="176"/>
       <c r="O23" s="177"/>
-      <c r="P23" s="601"/>
-      <c r="Q23" s="602"/>
-      <c r="R23" s="602"/>
-      <c r="S23" s="603"/>
+      <c r="P23" s="604"/>
+      <c r="Q23" s="605"/>
+      <c r="R23" s="605"/>
+      <c r="S23" s="606"/>
       <c r="T23" s="110"/>
       <c r="U23" s="178"/>
       <c r="V23" s="179"/>
@@ -6895,10 +6918,10 @@
       <c r="M24" s="187"/>
       <c r="N24" s="159"/>
       <c r="O24" s="177"/>
-      <c r="P24" s="604"/>
-      <c r="Q24" s="605"/>
-      <c r="R24" s="605"/>
-      <c r="S24" s="606"/>
+      <c r="P24" s="607"/>
+      <c r="Q24" s="608"/>
+      <c r="R24" s="608"/>
+      <c r="S24" s="609"/>
       <c r="T24" s="110"/>
       <c r="U24" s="178"/>
       <c r="V24" s="179"/>
@@ -7549,10 +7572,10 @@
       <c r="Q41" s="288"/>
       <c r="R41" s="301"/>
       <c r="S41" s="301"/>
-      <c r="T41" s="577"/>
-      <c r="U41" s="578"/>
-      <c r="V41" s="578"/>
-      <c r="W41" s="579"/>
+      <c r="T41" s="580"/>
+      <c r="U41" s="581"/>
+      <c r="V41" s="581"/>
+      <c r="W41" s="582"/>
       <c r="X41" s="302"/>
       <c r="Y41" s="303"/>
     </row>
@@ -7581,10 +7604,10 @@
       <c r="Q42" s="115"/>
       <c r="R42" s="301"/>
       <c r="S42" s="301"/>
-      <c r="T42" s="580"/>
-      <c r="U42" s="581"/>
-      <c r="V42" s="581"/>
-      <c r="W42" s="582"/>
+      <c r="T42" s="583"/>
+      <c r="U42" s="584"/>
+      <c r="V42" s="584"/>
+      <c r="W42" s="585"/>
       <c r="X42" s="302"/>
       <c r="Y42" s="303"/>
     </row>
@@ -8866,12 +8889,12 @@
         <v>28</v>
       </c>
       <c r="Q3" s="448"/>
-      <c r="R3" s="583" t="s">
+      <c r="R3" s="586" t="s">
         <v>306</v>
       </c>
-      <c r="S3" s="584"/>
-      <c r="T3" s="584"/>
-      <c r="U3" s="585"/>
+      <c r="S3" s="587"/>
+      <c r="T3" s="587"/>
+      <c r="U3" s="588"/>
       <c r="V3" s="27" t="s">
         <v>18</v>
       </c>
@@ -9581,12 +9604,12 @@
       <c r="Q17" s="497">
         <v>0.4</v>
       </c>
-      <c r="R17" s="586" t="s">
+      <c r="R17" s="589" t="s">
         <v>342</v>
       </c>
-      <c r="S17" s="587"/>
-      <c r="T17" s="588"/>
-      <c r="U17" s="589"/>
+      <c r="S17" s="590"/>
+      <c r="T17" s="591"/>
+      <c r="U17" s="592"/>
       <c r="V17" s="143" t="s">
         <v>88</v>
       </c>
@@ -9645,10 +9668,10 @@
         <f>P18+Q17</f>
         <v>1.2151933701657458</v>
       </c>
-      <c r="R18" s="590"/>
-      <c r="S18" s="591"/>
-      <c r="T18" s="591"/>
-      <c r="U18" s="592"/>
+      <c r="R18" s="593"/>
+      <c r="S18" s="594"/>
+      <c r="T18" s="594"/>
+      <c r="U18" s="595"/>
       <c r="V18" s="153" t="s">
         <v>89</v>
       </c>
@@ -9688,12 +9711,12 @@
       <c r="O19" s="511"/>
       <c r="P19" s="510"/>
       <c r="Q19" s="511"/>
-      <c r="R19" s="593" t="s">
+      <c r="R19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="S19" s="594"/>
-      <c r="T19" s="594"/>
-      <c r="U19" s="595"/>
+      <c r="S19" s="597"/>
+      <c r="T19" s="597"/>
+      <c r="U19" s="598"/>
       <c r="V19" s="161"/>
       <c r="W19" s="117"/>
       <c r="X19" s="162"/>
@@ -9771,11 +9794,11 @@
       <c r="P21" s="24"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="168"/>
-      <c r="S21" s="599" t="s">
+      <c r="S21" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="T21" s="599"/>
-      <c r="U21" s="600"/>
+      <c r="T21" s="602"/>
+      <c r="U21" s="603"/>
       <c r="V21" s="161"/>
       <c r="W21" s="117"/>
       <c r="X21" s="162"/>
@@ -9803,10 +9826,10 @@
       <c r="O22" s="504"/>
       <c r="P22" s="176"/>
       <c r="Q22" s="177"/>
-      <c r="R22" s="601"/>
-      <c r="S22" s="602"/>
-      <c r="T22" s="602"/>
-      <c r="U22" s="603"/>
+      <c r="R22" s="604"/>
+      <c r="S22" s="605"/>
+      <c r="T22" s="605"/>
+      <c r="U22" s="606"/>
       <c r="V22" s="110"/>
       <c r="W22" s="178"/>
       <c r="X22" s="179"/>
@@ -9837,10 +9860,10 @@
       <c r="O23" s="187"/>
       <c r="P23" s="159"/>
       <c r="Q23" s="177"/>
-      <c r="R23" s="604"/>
-      <c r="S23" s="605"/>
-      <c r="T23" s="605"/>
-      <c r="U23" s="606"/>
+      <c r="R23" s="607"/>
+      <c r="S23" s="608"/>
+      <c r="T23" s="608"/>
+      <c r="U23" s="609"/>
       <c r="V23" s="110"/>
       <c r="W23" s="178"/>
       <c r="X23" s="179"/>
@@ -10541,10 +10564,10 @@
       <c r="S40" s="288"/>
       <c r="T40" s="301"/>
       <c r="U40" s="301"/>
-      <c r="V40" s="577"/>
-      <c r="W40" s="578"/>
-      <c r="X40" s="578"/>
-      <c r="Y40" s="579"/>
+      <c r="V40" s="580"/>
+      <c r="W40" s="581"/>
+      <c r="X40" s="581"/>
+      <c r="Y40" s="582"/>
       <c r="Z40" s="302"/>
       <c r="AA40" s="303"/>
     </row>
@@ -10575,10 +10598,10 @@
       <c r="S41" s="115"/>
       <c r="T41" s="301"/>
       <c r="U41" s="301"/>
-      <c r="V41" s="580"/>
-      <c r="W41" s="581"/>
-      <c r="X41" s="581"/>
-      <c r="Y41" s="582"/>
+      <c r="V41" s="583"/>
+      <c r="W41" s="584"/>
+      <c r="X41" s="584"/>
+      <c r="Y41" s="585"/>
       <c r="Z41" s="302"/>
       <c r="AA41" s="303"/>
     </row>
@@ -11937,12 +11960,12 @@
         <v>28</v>
       </c>
       <c r="Q3" s="448"/>
-      <c r="R3" s="583" t="s">
+      <c r="R3" s="586" t="s">
         <v>306</v>
       </c>
-      <c r="S3" s="584"/>
-      <c r="T3" s="584"/>
-      <c r="U3" s="585"/>
+      <c r="S3" s="587"/>
+      <c r="T3" s="587"/>
+      <c r="U3" s="588"/>
       <c r="V3" s="27" t="s">
         <v>18</v>
       </c>
@@ -12640,12 +12663,12 @@
       <c r="Q17" s="497">
         <v>0.4</v>
       </c>
-      <c r="R17" s="586" t="s">
+      <c r="R17" s="589" t="s">
         <v>365</v>
       </c>
-      <c r="S17" s="587"/>
-      <c r="T17" s="588"/>
-      <c r="U17" s="589"/>
+      <c r="S17" s="590"/>
+      <c r="T17" s="591"/>
+      <c r="U17" s="592"/>
       <c r="V17" s="143" t="s">
         <v>88</v>
       </c>
@@ -12704,10 +12727,10 @@
         <f>P18+Q17</f>
         <v>1.1737265415549598</v>
       </c>
-      <c r="R18" s="590"/>
-      <c r="S18" s="591"/>
-      <c r="T18" s="591"/>
-      <c r="U18" s="592"/>
+      <c r="R18" s="593"/>
+      <c r="S18" s="594"/>
+      <c r="T18" s="594"/>
+      <c r="U18" s="595"/>
       <c r="V18" s="153" t="s">
         <v>89</v>
       </c>
@@ -12755,12 +12778,12 @@
       </c>
       <c r="P19" s="510"/>
       <c r="Q19" s="511"/>
-      <c r="R19" s="593" t="s">
+      <c r="R19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="S19" s="594"/>
-      <c r="T19" s="594"/>
-      <c r="U19" s="595"/>
+      <c r="S19" s="597"/>
+      <c r="T19" s="597"/>
+      <c r="U19" s="598"/>
       <c r="V19" s="161"/>
       <c r="W19" s="117"/>
       <c r="X19" s="162"/>
@@ -12837,11 +12860,11 @@
       <c r="P21" s="24"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="168"/>
-      <c r="S21" s="599" t="s">
+      <c r="S21" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="T21" s="599"/>
-      <c r="U21" s="600"/>
+      <c r="T21" s="602"/>
+      <c r="U21" s="603"/>
       <c r="V21" s="161"/>
       <c r="W21" s="117"/>
       <c r="X21" s="162"/>
@@ -12869,10 +12892,10 @@
       <c r="O22" s="504"/>
       <c r="P22" s="176"/>
       <c r="Q22" s="177"/>
-      <c r="R22" s="601"/>
-      <c r="S22" s="602"/>
-      <c r="T22" s="602"/>
-      <c r="U22" s="603"/>
+      <c r="R22" s="604"/>
+      <c r="S22" s="605"/>
+      <c r="T22" s="605"/>
+      <c r="U22" s="606"/>
       <c r="V22" s="110"/>
       <c r="W22" s="178"/>
       <c r="X22" s="179"/>
@@ -12903,10 +12926,10 @@
       <c r="O23" s="187"/>
       <c r="P23" s="159"/>
       <c r="Q23" s="177"/>
-      <c r="R23" s="604"/>
-      <c r="S23" s="605"/>
-      <c r="T23" s="605"/>
-      <c r="U23" s="606"/>
+      <c r="R23" s="607"/>
+      <c r="S23" s="608"/>
+      <c r="T23" s="608"/>
+      <c r="U23" s="609"/>
       <c r="V23" s="110"/>
       <c r="W23" s="178"/>
       <c r="X23" s="179"/>
@@ -13595,10 +13618,10 @@
       <c r="S40" s="288"/>
       <c r="T40" s="301"/>
       <c r="U40" s="301"/>
-      <c r="V40" s="577"/>
-      <c r="W40" s="578"/>
-      <c r="X40" s="578"/>
-      <c r="Y40" s="579"/>
+      <c r="V40" s="580"/>
+      <c r="W40" s="581"/>
+      <c r="X40" s="581"/>
+      <c r="Y40" s="582"/>
       <c r="Z40" s="302"/>
       <c r="AA40" s="303"/>
     </row>
@@ -13629,10 +13652,10 @@
       <c r="S41" s="115"/>
       <c r="T41" s="301"/>
       <c r="U41" s="301"/>
-      <c r="V41" s="580"/>
-      <c r="W41" s="581"/>
-      <c r="X41" s="581"/>
-      <c r="Y41" s="582"/>
+      <c r="V41" s="583"/>
+      <c r="W41" s="584"/>
+      <c r="X41" s="584"/>
+      <c r="Y41" s="585"/>
       <c r="Z41" s="302"/>
       <c r="AA41" s="303"/>
     </row>
@@ -14989,12 +15012,12 @@
         <v>28</v>
       </c>
       <c r="Q3" s="448"/>
-      <c r="R3" s="583" t="s">
+      <c r="R3" s="586" t="s">
         <v>306</v>
       </c>
-      <c r="S3" s="584"/>
-      <c r="T3" s="584"/>
-      <c r="U3" s="585"/>
+      <c r="S3" s="587"/>
+      <c r="T3" s="587"/>
+      <c r="U3" s="588"/>
       <c r="V3" s="27" t="s">
         <v>18</v>
       </c>
@@ -15693,12 +15716,12 @@
       <c r="Q17" s="497">
         <v>0.4</v>
       </c>
-      <c r="R17" s="586" t="s">
+      <c r="R17" s="589" t="s">
         <v>376</v>
       </c>
-      <c r="S17" s="587"/>
-      <c r="T17" s="588"/>
-      <c r="U17" s="589"/>
+      <c r="S17" s="590"/>
+      <c r="T17" s="591"/>
+      <c r="U17" s="592"/>
       <c r="V17" s="143" t="s">
         <v>88</v>
       </c>
@@ -15757,10 +15780,10 @@
         <f>P18+Q17</f>
         <v>1.4925133689839569</v>
       </c>
-      <c r="R18" s="590"/>
-      <c r="S18" s="591"/>
-      <c r="T18" s="591"/>
-      <c r="U18" s="592"/>
+      <c r="R18" s="593"/>
+      <c r="S18" s="594"/>
+      <c r="T18" s="594"/>
+      <c r="U18" s="595"/>
       <c r="V18" s="153" t="s">
         <v>89</v>
       </c>
@@ -15804,12 +15827,12 @@
       </c>
       <c r="P19" s="510"/>
       <c r="Q19" s="511"/>
-      <c r="R19" s="593" t="s">
+      <c r="R19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="S19" s="594"/>
-      <c r="T19" s="594"/>
-      <c r="U19" s="595"/>
+      <c r="S19" s="597"/>
+      <c r="T19" s="597"/>
+      <c r="U19" s="598"/>
       <c r="V19" s="161"/>
       <c r="W19" s="117"/>
       <c r="X19" s="162"/>
@@ -15895,11 +15918,11 @@
       <c r="P21" s="24"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="168"/>
-      <c r="S21" s="599" t="s">
+      <c r="S21" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="T21" s="599"/>
-      <c r="U21" s="600"/>
+      <c r="T21" s="602"/>
+      <c r="U21" s="603"/>
       <c r="V21" s="161"/>
       <c r="W21" s="117"/>
       <c r="X21" s="162"/>
@@ -15927,10 +15950,10 @@
       <c r="O22" s="504"/>
       <c r="P22" s="176"/>
       <c r="Q22" s="177"/>
-      <c r="R22" s="601"/>
-      <c r="S22" s="602"/>
-      <c r="T22" s="602"/>
-      <c r="U22" s="603"/>
+      <c r="R22" s="604"/>
+      <c r="S22" s="605"/>
+      <c r="T22" s="605"/>
+      <c r="U22" s="606"/>
       <c r="V22" s="110"/>
       <c r="W22" s="178"/>
       <c r="X22" s="179"/>
@@ -15961,10 +15984,10 @@
       <c r="O23" s="187"/>
       <c r="P23" s="159"/>
       <c r="Q23" s="177"/>
-      <c r="R23" s="604"/>
-      <c r="S23" s="605"/>
-      <c r="T23" s="605"/>
-      <c r="U23" s="606"/>
+      <c r="R23" s="607"/>
+      <c r="S23" s="608"/>
+      <c r="T23" s="608"/>
+      <c r="U23" s="609"/>
       <c r="V23" s="110"/>
       <c r="W23" s="178"/>
       <c r="X23" s="179"/>
@@ -16653,10 +16676,10 @@
       <c r="S40" s="288"/>
       <c r="T40" s="301"/>
       <c r="U40" s="301"/>
-      <c r="V40" s="577"/>
-      <c r="W40" s="578"/>
-      <c r="X40" s="578"/>
-      <c r="Y40" s="579"/>
+      <c r="V40" s="580"/>
+      <c r="W40" s="581"/>
+      <c r="X40" s="581"/>
+      <c r="Y40" s="582"/>
       <c r="Z40" s="302"/>
       <c r="AA40" s="303"/>
     </row>
@@ -16687,10 +16710,10 @@
       <c r="S41" s="115"/>
       <c r="T41" s="301"/>
       <c r="U41" s="301"/>
-      <c r="V41" s="580"/>
-      <c r="W41" s="581"/>
-      <c r="X41" s="581"/>
-      <c r="Y41" s="582"/>
+      <c r="V41" s="583"/>
+      <c r="W41" s="584"/>
+      <c r="X41" s="584"/>
+      <c r="Y41" s="585"/>
       <c r="Z41" s="302"/>
       <c r="AA41" s="303"/>
     </row>
@@ -17881,7 +17904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:BJ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J9" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -18049,12 +18072,12 @@
         <v>28</v>
       </c>
       <c r="Q3" s="448"/>
-      <c r="R3" s="583" t="s">
+      <c r="R3" s="586" t="s">
         <v>306</v>
       </c>
-      <c r="S3" s="584"/>
-      <c r="T3" s="584"/>
-      <c r="U3" s="585"/>
+      <c r="S3" s="587"/>
+      <c r="T3" s="587"/>
+      <c r="U3" s="588"/>
       <c r="V3" s="27" t="s">
         <v>18</v>
       </c>
@@ -18747,12 +18770,12 @@
       <c r="Q17" s="497">
         <v>0.4</v>
       </c>
-      <c r="R17" s="586" t="s">
+      <c r="R17" s="589" t="s">
         <v>397</v>
       </c>
-      <c r="S17" s="587"/>
-      <c r="T17" s="588"/>
-      <c r="U17" s="589"/>
+      <c r="S17" s="590"/>
+      <c r="T17" s="591"/>
+      <c r="U17" s="592"/>
       <c r="V17" s="143" t="s">
         <v>88</v>
       </c>
@@ -18811,10 +18834,10 @@
         <f>P18+Q17</f>
         <v>1.1048593350383631</v>
       </c>
-      <c r="R18" s="590"/>
-      <c r="S18" s="591"/>
-      <c r="T18" s="591"/>
-      <c r="U18" s="592"/>
+      <c r="R18" s="593"/>
+      <c r="S18" s="594"/>
+      <c r="T18" s="594"/>
+      <c r="U18" s="595"/>
       <c r="V18" s="153" t="s">
         <v>89</v>
       </c>
@@ -18866,12 +18889,12 @@
       </c>
       <c r="P19" s="510"/>
       <c r="Q19" s="511"/>
-      <c r="R19" s="593" t="s">
+      <c r="R19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="S19" s="594"/>
-      <c r="T19" s="594"/>
-      <c r="U19" s="595"/>
+      <c r="S19" s="597"/>
+      <c r="T19" s="597"/>
+      <c r="U19" s="598"/>
       <c r="V19" s="161"/>
       <c r="W19" s="117"/>
       <c r="X19" s="162"/>
@@ -18945,11 +18968,11 @@
       <c r="P21" s="24"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="168"/>
-      <c r="S21" s="599" t="s">
+      <c r="S21" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="T21" s="599"/>
-      <c r="U21" s="600"/>
+      <c r="T21" s="602"/>
+      <c r="U21" s="603"/>
       <c r="V21" s="161"/>
       <c r="W21" s="117"/>
       <c r="X21" s="162"/>
@@ -18977,10 +19000,10 @@
       <c r="O22" s="504"/>
       <c r="P22" s="176"/>
       <c r="Q22" s="177"/>
-      <c r="R22" s="601"/>
-      <c r="S22" s="602"/>
-      <c r="T22" s="602"/>
-      <c r="U22" s="603"/>
+      <c r="R22" s="604"/>
+      <c r="S22" s="605"/>
+      <c r="T22" s="605"/>
+      <c r="U22" s="606"/>
       <c r="V22" s="110"/>
       <c r="W22" s="178"/>
       <c r="X22" s="179"/>
@@ -19011,10 +19034,10 @@
       <c r="O23" s="187"/>
       <c r="P23" s="159"/>
       <c r="Q23" s="177"/>
-      <c r="R23" s="604"/>
-      <c r="S23" s="605"/>
-      <c r="T23" s="605"/>
-      <c r="U23" s="606"/>
+      <c r="R23" s="607"/>
+      <c r="S23" s="608"/>
+      <c r="T23" s="608"/>
+      <c r="U23" s="609"/>
       <c r="V23" s="110"/>
       <c r="W23" s="178"/>
       <c r="X23" s="179"/>
@@ -19703,10 +19726,10 @@
       <c r="S40" s="288"/>
       <c r="T40" s="301"/>
       <c r="U40" s="301"/>
-      <c r="V40" s="577"/>
-      <c r="W40" s="578"/>
-      <c r="X40" s="578"/>
-      <c r="Y40" s="579"/>
+      <c r="V40" s="580"/>
+      <c r="W40" s="581"/>
+      <c r="X40" s="581"/>
+      <c r="Y40" s="582"/>
       <c r="Z40" s="302"/>
       <c r="AA40" s="303"/>
     </row>
@@ -19737,10 +19760,10 @@
       <c r="S41" s="115"/>
       <c r="T41" s="301"/>
       <c r="U41" s="301"/>
-      <c r="V41" s="580"/>
-      <c r="W41" s="581"/>
-      <c r="X41" s="581"/>
-      <c r="Y41" s="582"/>
+      <c r="V41" s="583"/>
+      <c r="W41" s="584"/>
+      <c r="X41" s="584"/>
+      <c r="Y41" s="585"/>
       <c r="Z41" s="302"/>
       <c r="AA41" s="303"/>
     </row>
@@ -21099,12 +21122,12 @@
         <v>28</v>
       </c>
       <c r="Q3" s="448"/>
-      <c r="R3" s="583" t="s">
+      <c r="R3" s="586" t="s">
         <v>306</v>
       </c>
-      <c r="S3" s="584"/>
-      <c r="T3" s="584"/>
-      <c r="U3" s="585"/>
+      <c r="S3" s="587"/>
+      <c r="T3" s="587"/>
+      <c r="U3" s="588"/>
       <c r="V3" s="27" t="s">
         <v>18</v>
       </c>
@@ -21810,12 +21833,12 @@
       <c r="Q17" s="497">
         <v>0.4</v>
       </c>
-      <c r="R17" s="586" t="s">
+      <c r="R17" s="589" t="s">
         <v>404</v>
       </c>
-      <c r="S17" s="587"/>
-      <c r="T17" s="588"/>
-      <c r="U17" s="589"/>
+      <c r="S17" s="590"/>
+      <c r="T17" s="591"/>
+      <c r="U17" s="592"/>
       <c r="V17" s="143" t="s">
         <v>88</v>
       </c>
@@ -21874,10 +21897,10 @@
         <f>P18+Q17</f>
         <v>1.2174934725848563</v>
       </c>
-      <c r="R18" s="590"/>
-      <c r="S18" s="591"/>
-      <c r="T18" s="591"/>
-      <c r="U18" s="592"/>
+      <c r="R18" s="593"/>
+      <c r="S18" s="594"/>
+      <c r="T18" s="594"/>
+      <c r="U18" s="595"/>
       <c r="V18" s="153" t="s">
         <v>89</v>
       </c>
@@ -21929,12 +21952,12 @@
       </c>
       <c r="P19" s="510"/>
       <c r="Q19" s="511"/>
-      <c r="R19" s="593" t="s">
+      <c r="R19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="S19" s="594"/>
-      <c r="T19" s="594"/>
-      <c r="U19" s="595"/>
+      <c r="S19" s="597"/>
+      <c r="T19" s="597"/>
+      <c r="U19" s="598"/>
       <c r="V19" s="161"/>
       <c r="W19" s="117"/>
       <c r="X19" s="162"/>
@@ -22008,11 +22031,11 @@
       <c r="P21" s="24"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="168"/>
-      <c r="S21" s="599" t="s">
+      <c r="S21" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="T21" s="599"/>
-      <c r="U21" s="600"/>
+      <c r="T21" s="602"/>
+      <c r="U21" s="603"/>
       <c r="V21" s="161"/>
       <c r="W21" s="117"/>
       <c r="X21" s="162"/>
@@ -22040,10 +22063,10 @@
       <c r="O22" s="504"/>
       <c r="P22" s="176"/>
       <c r="Q22" s="177"/>
-      <c r="R22" s="601"/>
-      <c r="S22" s="602"/>
-      <c r="T22" s="602"/>
-      <c r="U22" s="603"/>
+      <c r="R22" s="604"/>
+      <c r="S22" s="605"/>
+      <c r="T22" s="605"/>
+      <c r="U22" s="606"/>
       <c r="V22" s="110"/>
       <c r="W22" s="178"/>
       <c r="X22" s="179"/>
@@ -22074,10 +22097,10 @@
       <c r="O23" s="187"/>
       <c r="P23" s="159"/>
       <c r="Q23" s="177"/>
-      <c r="R23" s="604"/>
-      <c r="S23" s="605"/>
-      <c r="T23" s="605"/>
-      <c r="U23" s="606"/>
+      <c r="R23" s="607"/>
+      <c r="S23" s="608"/>
+      <c r="T23" s="608"/>
+      <c r="U23" s="609"/>
       <c r="V23" s="110"/>
       <c r="W23" s="178"/>
       <c r="X23" s="179"/>
@@ -22766,10 +22789,10 @@
       <c r="S40" s="288"/>
       <c r="T40" s="301"/>
       <c r="U40" s="301"/>
-      <c r="V40" s="577"/>
-      <c r="W40" s="578"/>
-      <c r="X40" s="578"/>
-      <c r="Y40" s="579"/>
+      <c r="V40" s="580"/>
+      <c r="W40" s="581"/>
+      <c r="X40" s="581"/>
+      <c r="Y40" s="582"/>
       <c r="Z40" s="302"/>
       <c r="AA40" s="303"/>
     </row>
@@ -22800,10 +22823,10 @@
       <c r="S41" s="115"/>
       <c r="T41" s="301"/>
       <c r="U41" s="301"/>
-      <c r="V41" s="580"/>
-      <c r="W41" s="581"/>
-      <c r="X41" s="581"/>
-      <c r="Y41" s="582"/>
+      <c r="V41" s="583"/>
+      <c r="W41" s="584"/>
+      <c r="X41" s="584"/>
+      <c r="Y41" s="585"/>
       <c r="Z41" s="302"/>
       <c r="AA41" s="303"/>
     </row>
@@ -22841,7 +22864,7 @@
       <c r="Z42" s="306"/>
       <c r="AA42" s="303"/>
     </row>
-    <row r="43" spans="1:33" ht="108">
+    <row r="43" spans="1:33" ht="72">
       <c r="A43" s="310" t="s">
         <v>138</v>
       </c>
@@ -23994,7 +24017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:BJ101"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -24162,12 +24185,12 @@
         <v>28</v>
       </c>
       <c r="Q3" s="448"/>
-      <c r="R3" s="583" t="s">
+      <c r="R3" s="586" t="s">
         <v>306</v>
       </c>
-      <c r="S3" s="584"/>
-      <c r="T3" s="584"/>
-      <c r="U3" s="585"/>
+      <c r="S3" s="587"/>
+      <c r="T3" s="587"/>
+      <c r="U3" s="588"/>
       <c r="V3" s="27" t="s">
         <v>18</v>
       </c>
@@ -24855,12 +24878,12 @@
       <c r="Q17" s="497">
         <v>0.4</v>
       </c>
-      <c r="R17" s="586" t="s">
+      <c r="R17" s="589" t="s">
         <v>423</v>
       </c>
-      <c r="S17" s="587"/>
-      <c r="T17" s="588"/>
-      <c r="U17" s="589"/>
+      <c r="S17" s="590"/>
+      <c r="T17" s="591"/>
+      <c r="U17" s="592"/>
       <c r="V17" s="143" t="s">
         <v>88</v>
       </c>
@@ -24919,10 +24942,10 @@
         <f>P18+Q17</f>
         <v>1.3857142857142857</v>
       </c>
-      <c r="R18" s="590"/>
-      <c r="S18" s="591"/>
-      <c r="T18" s="591"/>
-      <c r="U18" s="592"/>
+      <c r="R18" s="593"/>
+      <c r="S18" s="594"/>
+      <c r="T18" s="594"/>
+      <c r="U18" s="595"/>
       <c r="V18" s="153" t="s">
         <v>89</v>
       </c>
@@ -24970,12 +24993,12 @@
       <c r="O19" s="504"/>
       <c r="P19" s="510"/>
       <c r="Q19" s="511"/>
-      <c r="R19" s="593" t="s">
+      <c r="R19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="S19" s="594"/>
-      <c r="T19" s="594"/>
-      <c r="U19" s="595"/>
+      <c r="S19" s="597"/>
+      <c r="T19" s="597"/>
+      <c r="U19" s="598"/>
       <c r="V19" s="161"/>
       <c r="W19" s="117"/>
       <c r="X19" s="162"/>
@@ -25057,11 +25080,11 @@
       <c r="P21" s="24"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="168"/>
-      <c r="S21" s="599" t="s">
+      <c r="S21" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="T21" s="599"/>
-      <c r="U21" s="600"/>
+      <c r="T21" s="602"/>
+      <c r="U21" s="603"/>
       <c r="V21" s="161"/>
       <c r="W21" s="117"/>
       <c r="X21" s="162"/>
@@ -25089,10 +25112,10 @@
       <c r="O22" s="504"/>
       <c r="P22" s="176"/>
       <c r="Q22" s="177"/>
-      <c r="R22" s="601"/>
-      <c r="S22" s="602"/>
-      <c r="T22" s="602"/>
-      <c r="U22" s="603"/>
+      <c r="R22" s="604"/>
+      <c r="S22" s="605"/>
+      <c r="T22" s="605"/>
+      <c r="U22" s="606"/>
       <c r="V22" s="110"/>
       <c r="W22" s="178"/>
       <c r="X22" s="179"/>
@@ -25123,10 +25146,10 @@
       <c r="O23" s="187"/>
       <c r="P23" s="159"/>
       <c r="Q23" s="177"/>
-      <c r="R23" s="604"/>
-      <c r="S23" s="605"/>
-      <c r="T23" s="605"/>
-      <c r="U23" s="606"/>
+      <c r="R23" s="607"/>
+      <c r="S23" s="608"/>
+      <c r="T23" s="608"/>
+      <c r="U23" s="609"/>
       <c r="V23" s="110"/>
       <c r="W23" s="178"/>
       <c r="X23" s="179"/>
@@ -25819,10 +25842,10 @@
       <c r="S40" s="288"/>
       <c r="T40" s="301"/>
       <c r="U40" s="301"/>
-      <c r="V40" s="577"/>
-      <c r="W40" s="578"/>
-      <c r="X40" s="578"/>
-      <c r="Y40" s="579"/>
+      <c r="V40" s="580"/>
+      <c r="W40" s="581"/>
+      <c r="X40" s="581"/>
+      <c r="Y40" s="582"/>
       <c r="Z40" s="302"/>
       <c r="AA40" s="303"/>
     </row>
@@ -25853,10 +25876,10 @@
       <c r="S41" s="115"/>
       <c r="T41" s="301"/>
       <c r="U41" s="301"/>
-      <c r="V41" s="580"/>
-      <c r="W41" s="581"/>
-      <c r="X41" s="581"/>
-      <c r="Y41" s="582"/>
+      <c r="V41" s="583"/>
+      <c r="W41" s="584"/>
+      <c r="X41" s="584"/>
+      <c r="Y41" s="585"/>
       <c r="Z41" s="302"/>
       <c r="AA41" s="303"/>
     </row>
@@ -25894,7 +25917,7 @@
       <c r="Z42" s="306"/>
       <c r="AA42" s="303"/>
     </row>
-    <row r="43" spans="1:33" ht="108">
+    <row r="43" spans="1:33" ht="72">
       <c r="A43" s="310" t="s">
         <v>138</v>
       </c>
@@ -27217,12 +27240,12 @@
         <v>28</v>
       </c>
       <c r="Q3" s="448"/>
-      <c r="R3" s="583" t="s">
+      <c r="R3" s="586" t="s">
         <v>306</v>
       </c>
-      <c r="S3" s="584"/>
-      <c r="T3" s="584"/>
-      <c r="U3" s="585"/>
+      <c r="S3" s="587"/>
+      <c r="T3" s="587"/>
+      <c r="U3" s="588"/>
       <c r="V3" s="27" t="s">
         <v>18</v>
       </c>
@@ -27909,12 +27932,12 @@
       <c r="Q17" s="497">
         <v>0.4</v>
       </c>
-      <c r="R17" s="586" t="s">
+      <c r="R17" s="589" t="s">
         <v>423</v>
       </c>
-      <c r="S17" s="587"/>
-      <c r="T17" s="588"/>
-      <c r="U17" s="589"/>
+      <c r="S17" s="590"/>
+      <c r="T17" s="591"/>
+      <c r="U17" s="592"/>
       <c r="V17" s="143" t="s">
         <v>88</v>
       </c>
@@ -27973,10 +27996,10 @@
         <f>P18+Q17</f>
         <v>1.111904761904762</v>
       </c>
-      <c r="R18" s="590"/>
-      <c r="S18" s="591"/>
-      <c r="T18" s="591"/>
-      <c r="U18" s="592"/>
+      <c r="R18" s="593"/>
+      <c r="S18" s="594"/>
+      <c r="T18" s="594"/>
+      <c r="U18" s="595"/>
       <c r="V18" s="153" t="s">
         <v>89</v>
       </c>
@@ -28024,12 +28047,12 @@
       <c r="O19" s="504"/>
       <c r="P19" s="510"/>
       <c r="Q19" s="511"/>
-      <c r="R19" s="593" t="s">
+      <c r="R19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="S19" s="594"/>
-      <c r="T19" s="594"/>
-      <c r="U19" s="595"/>
+      <c r="S19" s="597"/>
+      <c r="T19" s="597"/>
+      <c r="U19" s="598"/>
       <c r="V19" s="161"/>
       <c r="W19" s="117"/>
       <c r="X19" s="162"/>
@@ -28111,11 +28134,11 @@
       <c r="P21" s="24"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="168"/>
-      <c r="S21" s="599" t="s">
+      <c r="S21" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="T21" s="599"/>
-      <c r="U21" s="600"/>
+      <c r="T21" s="602"/>
+      <c r="U21" s="603"/>
       <c r="V21" s="161"/>
       <c r="W21" s="117"/>
       <c r="X21" s="162"/>
@@ -28143,10 +28166,10 @@
       <c r="O22" s="504"/>
       <c r="P22" s="176"/>
       <c r="Q22" s="177"/>
-      <c r="R22" s="601"/>
-      <c r="S22" s="602"/>
-      <c r="T22" s="602"/>
-      <c r="U22" s="603"/>
+      <c r="R22" s="604"/>
+      <c r="S22" s="605"/>
+      <c r="T22" s="605"/>
+      <c r="U22" s="606"/>
       <c r="V22" s="110"/>
       <c r="W22" s="178"/>
       <c r="X22" s="179"/>
@@ -28177,10 +28200,10 @@
       <c r="O23" s="187"/>
       <c r="P23" s="159"/>
       <c r="Q23" s="177"/>
-      <c r="R23" s="604"/>
-      <c r="S23" s="605"/>
-      <c r="T23" s="605"/>
-      <c r="U23" s="606"/>
+      <c r="R23" s="607"/>
+      <c r="S23" s="608"/>
+      <c r="T23" s="608"/>
+      <c r="U23" s="609"/>
       <c r="V23" s="110"/>
       <c r="W23" s="178"/>
       <c r="X23" s="179"/>
@@ -28869,10 +28892,10 @@
       <c r="S40" s="288"/>
       <c r="T40" s="301"/>
       <c r="U40" s="301"/>
-      <c r="V40" s="577"/>
-      <c r="W40" s="578"/>
-      <c r="X40" s="578"/>
-      <c r="Y40" s="579"/>
+      <c r="V40" s="580"/>
+      <c r="W40" s="581"/>
+      <c r="X40" s="581"/>
+      <c r="Y40" s="582"/>
       <c r="Z40" s="302"/>
       <c r="AA40" s="303"/>
     </row>
@@ -28903,10 +28926,10 @@
       <c r="S41" s="115"/>
       <c r="T41" s="301"/>
       <c r="U41" s="301"/>
-      <c r="V41" s="580"/>
-      <c r="W41" s="581"/>
-      <c r="X41" s="581"/>
-      <c r="Y41" s="582"/>
+      <c r="V41" s="583"/>
+      <c r="W41" s="584"/>
+      <c r="X41" s="584"/>
+      <c r="Y41" s="585"/>
       <c r="Z41" s="302"/>
       <c r="AA41" s="303"/>
     </row>
@@ -30097,8 +30120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:BJ101"/>
   <sheetViews>
-    <sheetView topLeftCell="M12" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="J5" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="35"/>
@@ -30265,12 +30288,12 @@
         <v>28</v>
       </c>
       <c r="Q3" s="448"/>
-      <c r="R3" s="583" t="s">
+      <c r="R3" s="586" t="s">
         <v>306</v>
       </c>
-      <c r="S3" s="584"/>
-      <c r="T3" s="584"/>
-      <c r="U3" s="585"/>
+      <c r="S3" s="587"/>
+      <c r="T3" s="587"/>
+      <c r="U3" s="588"/>
       <c r="V3" s="27" t="s">
         <v>18</v>
       </c>
@@ -30785,7 +30808,7 @@
       <c r="P13" s="563" t="s">
         <v>415</v>
       </c>
-      <c r="Q13" s="609" t="s">
+      <c r="Q13" s="579" t="s">
         <v>72</v>
       </c>
       <c r="R13" s="445" t="s">
@@ -30973,18 +30996,18 @@
       <c r="O17" s="495" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="607" t="s">
+      <c r="P17" s="577" t="s">
         <v>54</v>
       </c>
-      <c r="Q17" s="608">
+      <c r="Q17" s="578">
         <v>0.4</v>
       </c>
-      <c r="R17" s="586" t="s">
+      <c r="R17" s="589" t="s">
         <v>423</v>
       </c>
-      <c r="S17" s="587"/>
-      <c r="T17" s="588"/>
-      <c r="U17" s="589"/>
+      <c r="S17" s="590"/>
+      <c r="T17" s="591"/>
+      <c r="U17" s="592"/>
       <c r="V17" s="143" t="s">
         <v>88</v>
       </c>
@@ -31043,10 +31066,10 @@
         <f>P18+Q17</f>
         <v>1.3667525773195877</v>
       </c>
-      <c r="R18" s="590"/>
-      <c r="S18" s="591"/>
-      <c r="T18" s="591"/>
-      <c r="U18" s="592"/>
+      <c r="R18" s="593"/>
+      <c r="S18" s="594"/>
+      <c r="T18" s="594"/>
+      <c r="U18" s="595"/>
       <c r="V18" s="153" t="s">
         <v>89</v>
       </c>
@@ -31094,12 +31117,12 @@
       <c r="O19" s="504"/>
       <c r="P19" s="510"/>
       <c r="Q19" s="511"/>
-      <c r="R19" s="593" t="s">
+      <c r="R19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="S19" s="594"/>
-      <c r="T19" s="594"/>
-      <c r="U19" s="595"/>
+      <c r="S19" s="597"/>
+      <c r="T19" s="597"/>
+      <c r="U19" s="598"/>
       <c r="V19" s="161"/>
       <c r="W19" s="117"/>
       <c r="X19" s="162"/>
@@ -31181,11 +31204,11 @@
       <c r="P21" s="24"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="168"/>
-      <c r="S21" s="599" t="s">
+      <c r="S21" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="T21" s="599"/>
-      <c r="U21" s="600"/>
+      <c r="T21" s="602"/>
+      <c r="U21" s="603"/>
       <c r="V21" s="161"/>
       <c r="W21" s="117"/>
       <c r="X21" s="162"/>
@@ -31213,10 +31236,10 @@
       <c r="O22" s="504"/>
       <c r="P22" s="176"/>
       <c r="Q22" s="177"/>
-      <c r="R22" s="601"/>
-      <c r="S22" s="602"/>
-      <c r="T22" s="602"/>
-      <c r="U22" s="603"/>
+      <c r="R22" s="604"/>
+      <c r="S22" s="605"/>
+      <c r="T22" s="605"/>
+      <c r="U22" s="606"/>
       <c r="V22" s="110"/>
       <c r="W22" s="178"/>
       <c r="X22" s="179"/>
@@ -31247,10 +31270,10 @@
       <c r="O23" s="187"/>
       <c r="P23" s="159"/>
       <c r="Q23" s="177"/>
-      <c r="R23" s="604"/>
-      <c r="S23" s="605"/>
-      <c r="T23" s="605"/>
-      <c r="U23" s="606"/>
+      <c r="R23" s="607"/>
+      <c r="S23" s="608"/>
+      <c r="T23" s="608"/>
+      <c r="U23" s="609"/>
       <c r="V23" s="110"/>
       <c r="W23" s="178"/>
       <c r="X23" s="179"/>
@@ -31939,10 +31962,10 @@
       <c r="S40" s="288"/>
       <c r="T40" s="301"/>
       <c r="U40" s="301"/>
-      <c r="V40" s="577"/>
-      <c r="W40" s="578"/>
-      <c r="X40" s="578"/>
-      <c r="Y40" s="579"/>
+      <c r="V40" s="580"/>
+      <c r="W40" s="581"/>
+      <c r="X40" s="581"/>
+      <c r="Y40" s="582"/>
       <c r="Z40" s="302"/>
       <c r="AA40" s="303"/>
     </row>
@@ -31973,10 +31996,10 @@
       <c r="S41" s="115"/>
       <c r="T41" s="301"/>
       <c r="U41" s="301"/>
-      <c r="V41" s="580"/>
-      <c r="W41" s="581"/>
-      <c r="X41" s="581"/>
-      <c r="Y41" s="582"/>
+      <c r="V41" s="583"/>
+      <c r="W41" s="584"/>
+      <c r="X41" s="584"/>
+      <c r="Y41" s="585"/>
       <c r="Z41" s="302"/>
       <c r="AA41" s="303"/>
     </row>
@@ -32531,7 +32554,7 @@
     <row r="55" spans="1:27">
       <c r="A55" s="303"/>
       <c r="B55" s="361" t="s">
-        <v>158</v>
+        <v>486</v>
       </c>
       <c r="C55" s="362"/>
       <c r="D55" s="362"/>
@@ -33320,12 +33343,12 @@
         <v>16</v>
       </c>
       <c r="O3" s="26"/>
-      <c r="P3" s="583" t="s">
+      <c r="P3" s="586" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="584"/>
-      <c r="R3" s="584"/>
-      <c r="S3" s="585"/>
+      <c r="Q3" s="587"/>
+      <c r="R3" s="587"/>
+      <c r="S3" s="588"/>
       <c r="T3" s="27" t="s">
         <v>18</v>
       </c>
@@ -33969,12 +33992,12 @@
       <c r="O17" s="142">
         <v>0.4</v>
       </c>
-      <c r="P17" s="586" t="s">
+      <c r="P17" s="589" t="s">
         <v>195</v>
       </c>
-      <c r="Q17" s="587"/>
-      <c r="R17" s="588"/>
-      <c r="S17" s="589"/>
+      <c r="Q17" s="590"/>
+      <c r="R17" s="591"/>
+      <c r="S17" s="592"/>
       <c r="T17" s="143" t="s">
         <v>88</v>
       </c>
@@ -34028,10 +34051,10 @@
         <f>N18+O17</f>
         <v>1.348427672955975</v>
       </c>
-      <c r="P18" s="590"/>
-      <c r="Q18" s="591"/>
-      <c r="R18" s="591"/>
-      <c r="S18" s="592"/>
+      <c r="P18" s="593"/>
+      <c r="Q18" s="594"/>
+      <c r="R18" s="594"/>
+      <c r="S18" s="595"/>
       <c r="T18" s="153" t="s">
         <v>89</v>
       </c>
@@ -34069,12 +34092,12 @@
       <c r="M19" s="107"/>
       <c r="N19" s="56"/>
       <c r="O19" s="107"/>
-      <c r="P19" s="593" t="s">
+      <c r="P19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="Q19" s="594"/>
-      <c r="R19" s="594"/>
-      <c r="S19" s="595"/>
+      <c r="Q19" s="597"/>
+      <c r="R19" s="597"/>
+      <c r="S19" s="598"/>
       <c r="T19" s="161"/>
       <c r="U19" s="117"/>
       <c r="V19" s="162"/>
@@ -34112,10 +34135,10 @@
       <c r="M20" s="107"/>
       <c r="N20" s="24"/>
       <c r="O20" s="107"/>
-      <c r="P20" s="596"/>
-      <c r="Q20" s="597"/>
-      <c r="R20" s="597"/>
-      <c r="S20" s="598"/>
+      <c r="P20" s="599"/>
+      <c r="Q20" s="600"/>
+      <c r="R20" s="600"/>
+      <c r="S20" s="601"/>
       <c r="T20" s="161"/>
       <c r="U20" s="117"/>
       <c r="V20" s="162"/>
@@ -34185,11 +34208,11 @@
       <c r="N22" s="24"/>
       <c r="O22" s="20"/>
       <c r="P22" s="168"/>
-      <c r="Q22" s="599" t="s">
+      <c r="Q22" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="R22" s="599"/>
-      <c r="S22" s="600"/>
+      <c r="R22" s="602"/>
+      <c r="S22" s="603"/>
       <c r="T22" s="161"/>
       <c r="U22" s="117"/>
       <c r="V22" s="162"/>
@@ -34214,10 +34237,10 @@
       <c r="M23" s="175"/>
       <c r="N23" s="176"/>
       <c r="O23" s="177"/>
-      <c r="P23" s="601"/>
-      <c r="Q23" s="602"/>
-      <c r="R23" s="602"/>
-      <c r="S23" s="603"/>
+      <c r="P23" s="604"/>
+      <c r="Q23" s="605"/>
+      <c r="R23" s="605"/>
+      <c r="S23" s="606"/>
       <c r="T23" s="110"/>
       <c r="U23" s="178"/>
       <c r="V23" s="179"/>
@@ -34247,10 +34270,10 @@
       <c r="M24" s="187"/>
       <c r="N24" s="159"/>
       <c r="O24" s="177"/>
-      <c r="P24" s="604"/>
-      <c r="Q24" s="605"/>
-      <c r="R24" s="605"/>
-      <c r="S24" s="606"/>
+      <c r="P24" s="607"/>
+      <c r="Q24" s="608"/>
+      <c r="R24" s="608"/>
+      <c r="S24" s="609"/>
       <c r="T24" s="110"/>
       <c r="U24" s="178"/>
       <c r="V24" s="179"/>
@@ -34905,10 +34928,10 @@
       <c r="Q41" s="288"/>
       <c r="R41" s="301"/>
       <c r="S41" s="301"/>
-      <c r="T41" s="577"/>
-      <c r="U41" s="578"/>
-      <c r="V41" s="578"/>
-      <c r="W41" s="579"/>
+      <c r="T41" s="580"/>
+      <c r="U41" s="581"/>
+      <c r="V41" s="581"/>
+      <c r="W41" s="582"/>
       <c r="X41" s="302"/>
       <c r="Y41" s="303"/>
     </row>
@@ -34937,10 +34960,10 @@
       <c r="Q42" s="115"/>
       <c r="R42" s="301"/>
       <c r="S42" s="301"/>
-      <c r="T42" s="580"/>
-      <c r="U42" s="581"/>
-      <c r="V42" s="581"/>
-      <c r="W42" s="582"/>
+      <c r="T42" s="583"/>
+      <c r="U42" s="584"/>
+      <c r="V42" s="584"/>
+      <c r="W42" s="585"/>
       <c r="X42" s="302"/>
       <c r="Y42" s="303"/>
     </row>
@@ -36210,12 +36233,12 @@
         <v>28</v>
       </c>
       <c r="O3" s="26"/>
-      <c r="P3" s="583" t="s">
+      <c r="P3" s="586" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="584"/>
-      <c r="R3" s="584"/>
-      <c r="S3" s="585"/>
+      <c r="Q3" s="587"/>
+      <c r="R3" s="587"/>
+      <c r="S3" s="588"/>
       <c r="T3" s="27" t="s">
         <v>18</v>
       </c>
@@ -36872,12 +36895,12 @@
       <c r="O17" s="142">
         <v>0.4</v>
       </c>
-      <c r="P17" s="586" t="s">
+      <c r="P17" s="589" t="s">
         <v>195</v>
       </c>
-      <c r="Q17" s="587"/>
-      <c r="R17" s="588"/>
-      <c r="S17" s="589"/>
+      <c r="Q17" s="590"/>
+      <c r="R17" s="591"/>
+      <c r="S17" s="592"/>
       <c r="T17" s="143" t="s">
         <v>88</v>
       </c>
@@ -36931,10 +36954,10 @@
         <f>N18+O17</f>
         <v>1.2326283987915407</v>
       </c>
-      <c r="P18" s="590"/>
-      <c r="Q18" s="591"/>
-      <c r="R18" s="591"/>
-      <c r="S18" s="592"/>
+      <c r="P18" s="593"/>
+      <c r="Q18" s="594"/>
+      <c r="R18" s="594"/>
+      <c r="S18" s="595"/>
       <c r="T18" s="153" t="s">
         <v>89</v>
       </c>
@@ -36964,12 +36987,12 @@
       <c r="M19" s="107"/>
       <c r="N19" s="56"/>
       <c r="O19" s="107"/>
-      <c r="P19" s="593" t="s">
+      <c r="P19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="Q19" s="594"/>
-      <c r="R19" s="594"/>
-      <c r="S19" s="595"/>
+      <c r="Q19" s="597"/>
+      <c r="R19" s="597"/>
+      <c r="S19" s="598"/>
       <c r="T19" s="161"/>
       <c r="U19" s="117"/>
       <c r="V19" s="162"/>
@@ -37035,11 +37058,11 @@
       <c r="N21" s="24"/>
       <c r="O21" s="20"/>
       <c r="P21" s="168"/>
-      <c r="Q21" s="599" t="s">
+      <c r="Q21" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="R21" s="599"/>
-      <c r="S21" s="600"/>
+      <c r="R21" s="602"/>
+      <c r="S21" s="603"/>
       <c r="T21" s="161"/>
       <c r="U21" s="117"/>
       <c r="V21" s="162"/>
@@ -37064,10 +37087,10 @@
       <c r="M22" s="175"/>
       <c r="N22" s="176"/>
       <c r="O22" s="177"/>
-      <c r="P22" s="601"/>
-      <c r="Q22" s="602"/>
-      <c r="R22" s="602"/>
-      <c r="S22" s="603"/>
+      <c r="P22" s="604"/>
+      <c r="Q22" s="605"/>
+      <c r="R22" s="605"/>
+      <c r="S22" s="606"/>
       <c r="T22" s="110"/>
       <c r="U22" s="178"/>
       <c r="V22" s="179"/>
@@ -37097,10 +37120,10 @@
       <c r="M23" s="187"/>
       <c r="N23" s="159"/>
       <c r="O23" s="177"/>
-      <c r="P23" s="604"/>
-      <c r="Q23" s="605"/>
-      <c r="R23" s="605"/>
-      <c r="S23" s="606"/>
+      <c r="P23" s="607"/>
+      <c r="Q23" s="608"/>
+      <c r="R23" s="608"/>
+      <c r="S23" s="609"/>
       <c r="T23" s="110"/>
       <c r="U23" s="178"/>
       <c r="V23" s="179"/>
@@ -37756,10 +37779,10 @@
       <c r="Q40" s="288"/>
       <c r="R40" s="301"/>
       <c r="S40" s="301"/>
-      <c r="T40" s="577"/>
-      <c r="U40" s="578"/>
-      <c r="V40" s="578"/>
-      <c r="W40" s="579"/>
+      <c r="T40" s="580"/>
+      <c r="U40" s="581"/>
+      <c r="V40" s="581"/>
+      <c r="W40" s="582"/>
       <c r="X40" s="302"/>
       <c r="Y40" s="303"/>
     </row>
@@ -37788,10 +37811,10 @@
       <c r="Q41" s="115"/>
       <c r="R41" s="301"/>
       <c r="S41" s="301"/>
-      <c r="T41" s="580"/>
-      <c r="U41" s="581"/>
-      <c r="V41" s="581"/>
-      <c r="W41" s="582"/>
+      <c r="T41" s="583"/>
+      <c r="U41" s="584"/>
+      <c r="V41" s="584"/>
+      <c r="W41" s="585"/>
       <c r="X41" s="302"/>
       <c r="Y41" s="303"/>
     </row>
@@ -39064,12 +39087,12 @@
         <v>28</v>
       </c>
       <c r="O3" s="26"/>
-      <c r="P3" s="583" t="s">
+      <c r="P3" s="586" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="584"/>
-      <c r="R3" s="584"/>
-      <c r="S3" s="585"/>
+      <c r="Q3" s="587"/>
+      <c r="R3" s="587"/>
+      <c r="S3" s="588"/>
       <c r="T3" s="27" t="s">
         <v>18</v>
       </c>
@@ -39725,12 +39748,12 @@
       <c r="O17" s="142">
         <v>0.4</v>
       </c>
-      <c r="P17" s="586" t="s">
+      <c r="P17" s="589" t="s">
         <v>195</v>
       </c>
-      <c r="Q17" s="587"/>
-      <c r="R17" s="588"/>
-      <c r="S17" s="589"/>
+      <c r="Q17" s="590"/>
+      <c r="R17" s="591"/>
+      <c r="S17" s="592"/>
       <c r="T17" s="143" t="s">
         <v>88</v>
       </c>
@@ -39784,10 +39807,10 @@
         <f>N18+O17</f>
         <v>1.1433701657458564</v>
       </c>
-      <c r="P18" s="590"/>
-      <c r="Q18" s="591"/>
-      <c r="R18" s="591"/>
-      <c r="S18" s="592"/>
+      <c r="P18" s="593"/>
+      <c r="Q18" s="594"/>
+      <c r="R18" s="594"/>
+      <c r="S18" s="595"/>
       <c r="T18" s="153" t="s">
         <v>89</v>
       </c>
@@ -39829,12 +39852,12 @@
       <c r="M19" s="107"/>
       <c r="N19" s="56"/>
       <c r="O19" s="107"/>
-      <c r="P19" s="593" t="s">
+      <c r="P19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="Q19" s="594"/>
-      <c r="R19" s="594"/>
-      <c r="S19" s="595"/>
+      <c r="Q19" s="597"/>
+      <c r="R19" s="597"/>
+      <c r="S19" s="598"/>
       <c r="T19" s="161"/>
       <c r="U19" s="117"/>
       <c r="V19" s="162"/>
@@ -39908,11 +39931,11 @@
       <c r="N21" s="24"/>
       <c r="O21" s="20"/>
       <c r="P21" s="168"/>
-      <c r="Q21" s="599" t="s">
+      <c r="Q21" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="R21" s="599"/>
-      <c r="S21" s="600"/>
+      <c r="R21" s="602"/>
+      <c r="S21" s="603"/>
       <c r="T21" s="161"/>
       <c r="U21" s="117"/>
       <c r="V21" s="162"/>
@@ -39937,10 +39960,10 @@
       <c r="M22" s="175"/>
       <c r="N22" s="176"/>
       <c r="O22" s="177"/>
-      <c r="P22" s="601"/>
-      <c r="Q22" s="602"/>
-      <c r="R22" s="602"/>
-      <c r="S22" s="603"/>
+      <c r="P22" s="604"/>
+      <c r="Q22" s="605"/>
+      <c r="R22" s="605"/>
+      <c r="S22" s="606"/>
       <c r="T22" s="110"/>
       <c r="U22" s="178"/>
       <c r="V22" s="179"/>
@@ -39970,10 +39993,10 @@
       <c r="M23" s="187"/>
       <c r="N23" s="159"/>
       <c r="O23" s="177"/>
-      <c r="P23" s="604"/>
-      <c r="Q23" s="605"/>
-      <c r="R23" s="605"/>
-      <c r="S23" s="606"/>
+      <c r="P23" s="607"/>
+      <c r="Q23" s="608"/>
+      <c r="R23" s="608"/>
+      <c r="S23" s="609"/>
       <c r="T23" s="110"/>
       <c r="U23" s="178"/>
       <c r="V23" s="179"/>
@@ -40621,10 +40644,10 @@
       <c r="Q40" s="288"/>
       <c r="R40" s="301"/>
       <c r="S40" s="301"/>
-      <c r="T40" s="577"/>
-      <c r="U40" s="578"/>
-      <c r="V40" s="578"/>
-      <c r="W40" s="579"/>
+      <c r="T40" s="580"/>
+      <c r="U40" s="581"/>
+      <c r="V40" s="581"/>
+      <c r="W40" s="582"/>
       <c r="X40" s="302"/>
       <c r="Y40" s="303"/>
     </row>
@@ -40653,10 +40676,10 @@
       <c r="Q41" s="115"/>
       <c r="R41" s="301"/>
       <c r="S41" s="301"/>
-      <c r="T41" s="580"/>
-      <c r="U41" s="581"/>
-      <c r="V41" s="581"/>
-      <c r="W41" s="582"/>
+      <c r="T41" s="583"/>
+      <c r="U41" s="584"/>
+      <c r="V41" s="584"/>
+      <c r="W41" s="585"/>
       <c r="X41" s="302"/>
       <c r="Y41" s="303"/>
     </row>
@@ -41929,12 +41952,12 @@
         <v>28</v>
       </c>
       <c r="O3" s="26"/>
-      <c r="P3" s="583" t="s">
+      <c r="P3" s="586" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="584"/>
-      <c r="R3" s="584"/>
-      <c r="S3" s="585"/>
+      <c r="Q3" s="587"/>
+      <c r="R3" s="587"/>
+      <c r="S3" s="588"/>
       <c r="T3" s="27" t="s">
         <v>18</v>
       </c>
@@ -42582,12 +42605,12 @@
       <c r="O17" s="142">
         <v>0.4</v>
       </c>
-      <c r="P17" s="586" t="s">
+      <c r="P17" s="589" t="s">
         <v>195</v>
       </c>
-      <c r="Q17" s="587"/>
-      <c r="R17" s="588"/>
-      <c r="S17" s="589"/>
+      <c r="Q17" s="590"/>
+      <c r="R17" s="591"/>
+      <c r="S17" s="592"/>
       <c r="T17" s="143" t="s">
         <v>88</v>
       </c>
@@ -42641,10 +42664,10 @@
         <f>N18+O17</f>
         <v>1.1454293628808865</v>
       </c>
-      <c r="P18" s="590"/>
-      <c r="Q18" s="591"/>
-      <c r="R18" s="591"/>
-      <c r="S18" s="592"/>
+      <c r="P18" s="593"/>
+      <c r="Q18" s="594"/>
+      <c r="R18" s="594"/>
+      <c r="S18" s="595"/>
       <c r="T18" s="153" t="s">
         <v>89</v>
       </c>
@@ -42674,12 +42697,12 @@
       <c r="M19" s="107"/>
       <c r="N19" s="56"/>
       <c r="O19" s="107"/>
-      <c r="P19" s="593" t="s">
+      <c r="P19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="Q19" s="594"/>
-      <c r="R19" s="594"/>
-      <c r="S19" s="595"/>
+      <c r="Q19" s="597"/>
+      <c r="R19" s="597"/>
+      <c r="S19" s="598"/>
       <c r="T19" s="161"/>
       <c r="U19" s="117"/>
       <c r="V19" s="162"/>
@@ -42745,11 +42768,11 @@
       <c r="N21" s="24"/>
       <c r="O21" s="20"/>
       <c r="P21" s="168"/>
-      <c r="Q21" s="599" t="s">
+      <c r="Q21" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="R21" s="599"/>
-      <c r="S21" s="600"/>
+      <c r="R21" s="602"/>
+      <c r="S21" s="603"/>
       <c r="T21" s="161"/>
       <c r="U21" s="117"/>
       <c r="V21" s="162"/>
@@ -42774,10 +42797,10 @@
       <c r="M22" s="175"/>
       <c r="N22" s="176"/>
       <c r="O22" s="177"/>
-      <c r="P22" s="601"/>
-      <c r="Q22" s="602"/>
-      <c r="R22" s="602"/>
-      <c r="S22" s="603"/>
+      <c r="P22" s="604"/>
+      <c r="Q22" s="605"/>
+      <c r="R22" s="605"/>
+      <c r="S22" s="606"/>
       <c r="T22" s="110"/>
       <c r="U22" s="178"/>
       <c r="V22" s="179"/>
@@ -42807,10 +42830,10 @@
       <c r="M23" s="187"/>
       <c r="N23" s="159"/>
       <c r="O23" s="177"/>
-      <c r="P23" s="604"/>
-      <c r="Q23" s="605"/>
-      <c r="R23" s="605"/>
-      <c r="S23" s="606"/>
+      <c r="P23" s="607"/>
+      <c r="Q23" s="608"/>
+      <c r="R23" s="608"/>
+      <c r="S23" s="609"/>
       <c r="T23" s="110"/>
       <c r="U23" s="178"/>
       <c r="V23" s="179"/>
@@ -43458,10 +43481,10 @@
       <c r="Q40" s="288"/>
       <c r="R40" s="301"/>
       <c r="S40" s="301"/>
-      <c r="T40" s="577"/>
-      <c r="U40" s="578"/>
-      <c r="V40" s="578"/>
-      <c r="W40" s="579"/>
+      <c r="T40" s="580"/>
+      <c r="U40" s="581"/>
+      <c r="V40" s="581"/>
+      <c r="W40" s="582"/>
       <c r="X40" s="302"/>
       <c r="Y40" s="303"/>
     </row>
@@ -43490,10 +43513,10 @@
       <c r="Q41" s="115"/>
       <c r="R41" s="301"/>
       <c r="S41" s="301"/>
-      <c r="T41" s="580"/>
-      <c r="U41" s="581"/>
-      <c r="V41" s="581"/>
-      <c r="W41" s="582"/>
+      <c r="T41" s="583"/>
+      <c r="U41" s="584"/>
+      <c r="V41" s="584"/>
+      <c r="W41" s="585"/>
       <c r="X41" s="302"/>
       <c r="Y41" s="303"/>
     </row>
@@ -44763,12 +44786,12 @@
         <v>16</v>
       </c>
       <c r="O3" s="20"/>
-      <c r="P3" s="583" t="s">
+      <c r="P3" s="586" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="584"/>
-      <c r="R3" s="584"/>
-      <c r="S3" s="585"/>
+      <c r="Q3" s="587"/>
+      <c r="R3" s="587"/>
+      <c r="S3" s="588"/>
       <c r="T3" s="27" t="s">
         <v>18</v>
       </c>
@@ -45416,12 +45439,12 @@
       <c r="O17" s="142">
         <v>0.4</v>
       </c>
-      <c r="P17" s="586" t="s">
+      <c r="P17" s="589" t="s">
         <v>195</v>
       </c>
-      <c r="Q17" s="587"/>
-      <c r="R17" s="588"/>
-      <c r="S17" s="589"/>
+      <c r="Q17" s="590"/>
+      <c r="R17" s="591"/>
+      <c r="S17" s="592"/>
       <c r="T17" s="143" t="s">
         <v>88</v>
       </c>
@@ -45475,10 +45498,10 @@
         <f>N18+O17</f>
         <v>1.1904432132963989</v>
       </c>
-      <c r="P18" s="590"/>
-      <c r="Q18" s="591"/>
-      <c r="R18" s="591"/>
-      <c r="S18" s="592"/>
+      <c r="P18" s="593"/>
+      <c r="Q18" s="594"/>
+      <c r="R18" s="594"/>
+      <c r="S18" s="595"/>
       <c r="T18" s="153" t="s">
         <v>89</v>
       </c>
@@ -45520,12 +45543,12 @@
       <c r="M19" s="107"/>
       <c r="N19" s="56"/>
       <c r="O19" s="107"/>
-      <c r="P19" s="593" t="s">
+      <c r="P19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="Q19" s="594"/>
-      <c r="R19" s="594"/>
-      <c r="S19" s="595"/>
+      <c r="Q19" s="597"/>
+      <c r="R19" s="597"/>
+      <c r="S19" s="598"/>
       <c r="T19" s="161"/>
       <c r="U19" s="117"/>
       <c r="V19" s="162"/>
@@ -45567,10 +45590,10 @@
       <c r="M20" s="107"/>
       <c r="N20" s="24"/>
       <c r="O20" s="107"/>
-      <c r="P20" s="596"/>
-      <c r="Q20" s="597"/>
-      <c r="R20" s="597"/>
-      <c r="S20" s="598"/>
+      <c r="P20" s="599"/>
+      <c r="Q20" s="600"/>
+      <c r="R20" s="600"/>
+      <c r="S20" s="601"/>
       <c r="T20" s="161"/>
       <c r="U20" s="117"/>
       <c r="V20" s="162"/>
@@ -45630,11 +45653,11 @@
       <c r="N22" s="24"/>
       <c r="O22" s="20"/>
       <c r="P22" s="168"/>
-      <c r="Q22" s="599" t="s">
+      <c r="Q22" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="R22" s="599"/>
-      <c r="S22" s="600"/>
+      <c r="R22" s="602"/>
+      <c r="S22" s="603"/>
       <c r="T22" s="161"/>
       <c r="U22" s="117"/>
       <c r="V22" s="162"/>
@@ -45661,10 +45684,10 @@
       <c r="M23" s="175"/>
       <c r="N23" s="176"/>
       <c r="O23" s="177"/>
-      <c r="P23" s="601"/>
-      <c r="Q23" s="602"/>
-      <c r="R23" s="602"/>
-      <c r="S23" s="603"/>
+      <c r="P23" s="604"/>
+      <c r="Q23" s="605"/>
+      <c r="R23" s="605"/>
+      <c r="S23" s="606"/>
       <c r="T23" s="110"/>
       <c r="U23" s="178"/>
       <c r="V23" s="179"/>
@@ -45694,10 +45717,10 @@
       <c r="M24" s="187"/>
       <c r="N24" s="159"/>
       <c r="O24" s="177"/>
-      <c r="P24" s="604"/>
-      <c r="Q24" s="605"/>
-      <c r="R24" s="605"/>
-      <c r="S24" s="606"/>
+      <c r="P24" s="607"/>
+      <c r="Q24" s="608"/>
+      <c r="R24" s="608"/>
+      <c r="S24" s="609"/>
       <c r="T24" s="110"/>
       <c r="U24" s="178"/>
       <c r="V24" s="179"/>
@@ -46340,10 +46363,10 @@
       <c r="Q41" s="288"/>
       <c r="R41" s="301"/>
       <c r="S41" s="301"/>
-      <c r="T41" s="577"/>
-      <c r="U41" s="578"/>
-      <c r="V41" s="578"/>
-      <c r="W41" s="579"/>
+      <c r="T41" s="580"/>
+      <c r="U41" s="581"/>
+      <c r="V41" s="581"/>
+      <c r="W41" s="582"/>
       <c r="X41" s="302"/>
       <c r="Y41" s="303"/>
     </row>
@@ -46372,10 +46395,10 @@
       <c r="Q42" s="115"/>
       <c r="R42" s="301"/>
       <c r="S42" s="301"/>
-      <c r="T42" s="580"/>
-      <c r="U42" s="581"/>
-      <c r="V42" s="581"/>
-      <c r="W42" s="582"/>
+      <c r="T42" s="583"/>
+      <c r="U42" s="584"/>
+      <c r="V42" s="584"/>
+      <c r="W42" s="585"/>
       <c r="X42" s="302"/>
       <c r="Y42" s="303"/>
     </row>
@@ -47644,12 +47667,12 @@
         <v>16</v>
       </c>
       <c r="O3" s="20"/>
-      <c r="P3" s="583" t="s">
+      <c r="P3" s="586" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="584"/>
-      <c r="R3" s="584"/>
-      <c r="S3" s="585"/>
+      <c r="Q3" s="587"/>
+      <c r="R3" s="587"/>
+      <c r="S3" s="588"/>
       <c r="T3" s="27" t="s">
         <v>18</v>
       </c>
@@ -48298,12 +48321,12 @@
       <c r="O17" s="142">
         <v>0.4</v>
       </c>
-      <c r="P17" s="586" t="s">
+      <c r="P17" s="589" t="s">
         <v>195</v>
       </c>
-      <c r="Q17" s="587"/>
-      <c r="R17" s="588"/>
-      <c r="S17" s="589"/>
+      <c r="Q17" s="590"/>
+      <c r="R17" s="591"/>
+      <c r="S17" s="592"/>
       <c r="T17" s="143" t="s">
         <v>88</v>
       </c>
@@ -48357,10 +48380,10 @@
         <f>N18+O17</f>
         <v>1.2904624277456649</v>
       </c>
-      <c r="P18" s="590"/>
-      <c r="Q18" s="591"/>
-      <c r="R18" s="591"/>
-      <c r="S18" s="592"/>
+      <c r="P18" s="593"/>
+      <c r="Q18" s="594"/>
+      <c r="R18" s="594"/>
+      <c r="S18" s="595"/>
       <c r="T18" s="153" t="s">
         <v>89</v>
       </c>
@@ -48390,12 +48413,12 @@
       <c r="M19" s="107"/>
       <c r="N19" s="56"/>
       <c r="O19" s="107"/>
-      <c r="P19" s="593" t="s">
+      <c r="P19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="Q19" s="594"/>
-      <c r="R19" s="594"/>
-      <c r="S19" s="595"/>
+      <c r="Q19" s="597"/>
+      <c r="R19" s="597"/>
+      <c r="S19" s="598"/>
       <c r="T19" s="161"/>
       <c r="U19" s="117"/>
       <c r="V19" s="162"/>
@@ -48429,10 +48452,10 @@
       <c r="M20" s="107"/>
       <c r="N20" s="24"/>
       <c r="O20" s="107"/>
-      <c r="P20" s="596"/>
-      <c r="Q20" s="597"/>
-      <c r="R20" s="597"/>
-      <c r="S20" s="598"/>
+      <c r="P20" s="599"/>
+      <c r="Q20" s="600"/>
+      <c r="R20" s="600"/>
+      <c r="S20" s="601"/>
       <c r="T20" s="161"/>
       <c r="U20" s="117"/>
       <c r="V20" s="162"/>
@@ -48492,11 +48515,11 @@
       <c r="N22" s="24"/>
       <c r="O22" s="20"/>
       <c r="P22" s="168"/>
-      <c r="Q22" s="599" t="s">
+      <c r="Q22" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="R22" s="599"/>
-      <c r="S22" s="600"/>
+      <c r="R22" s="602"/>
+      <c r="S22" s="603"/>
       <c r="T22" s="161"/>
       <c r="U22" s="117"/>
       <c r="V22" s="162"/>
@@ -48523,10 +48546,10 @@
       <c r="M23" s="175"/>
       <c r="N23" s="176"/>
       <c r="O23" s="177"/>
-      <c r="P23" s="601"/>
-      <c r="Q23" s="602"/>
-      <c r="R23" s="602"/>
-      <c r="S23" s="603"/>
+      <c r="P23" s="604"/>
+      <c r="Q23" s="605"/>
+      <c r="R23" s="605"/>
+      <c r="S23" s="606"/>
       <c r="T23" s="110"/>
       <c r="U23" s="178"/>
       <c r="V23" s="179"/>
@@ -48556,10 +48579,10 @@
       <c r="M24" s="187"/>
       <c r="N24" s="159"/>
       <c r="O24" s="177"/>
-      <c r="P24" s="604"/>
-      <c r="Q24" s="605"/>
-      <c r="R24" s="605"/>
-      <c r="S24" s="606"/>
+      <c r="P24" s="607"/>
+      <c r="Q24" s="608"/>
+      <c r="R24" s="608"/>
+      <c r="S24" s="609"/>
       <c r="T24" s="110"/>
       <c r="U24" s="178"/>
       <c r="V24" s="179"/>
@@ -49209,10 +49232,10 @@
       <c r="Q41" s="288"/>
       <c r="R41" s="301"/>
       <c r="S41" s="301"/>
-      <c r="T41" s="577"/>
-      <c r="U41" s="578"/>
-      <c r="V41" s="578"/>
-      <c r="W41" s="579"/>
+      <c r="T41" s="580"/>
+      <c r="U41" s="581"/>
+      <c r="V41" s="581"/>
+      <c r="W41" s="582"/>
       <c r="X41" s="302"/>
       <c r="Y41" s="303"/>
     </row>
@@ -49241,10 +49264,10 @@
       <c r="Q42" s="115"/>
       <c r="R42" s="301"/>
       <c r="S42" s="301"/>
-      <c r="T42" s="580"/>
-      <c r="U42" s="581"/>
-      <c r="V42" s="581"/>
-      <c r="W42" s="582"/>
+      <c r="T42" s="583"/>
+      <c r="U42" s="584"/>
+      <c r="V42" s="584"/>
+      <c r="W42" s="585"/>
       <c r="X42" s="302"/>
       <c r="Y42" s="303"/>
     </row>
@@ -50516,12 +50539,12 @@
         <v>16</v>
       </c>
       <c r="O3" s="20"/>
-      <c r="P3" s="583" t="s">
+      <c r="P3" s="586" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="584"/>
-      <c r="R3" s="584"/>
-      <c r="S3" s="585"/>
+      <c r="Q3" s="587"/>
+      <c r="R3" s="587"/>
+      <c r="S3" s="588"/>
       <c r="T3" s="27" t="s">
         <v>18</v>
       </c>
@@ -51186,12 +51209,12 @@
       <c r="O17" s="142">
         <v>0.4</v>
       </c>
-      <c r="P17" s="586" t="s">
+      <c r="P17" s="589" t="s">
         <v>195</v>
       </c>
-      <c r="Q17" s="587"/>
-      <c r="R17" s="588"/>
-      <c r="S17" s="589"/>
+      <c r="Q17" s="590"/>
+      <c r="R17" s="591"/>
+      <c r="S17" s="592"/>
       <c r="T17" s="143" t="s">
         <v>88</v>
       </c>
@@ -51245,10 +51268,10 @@
         <f>N18+O17</f>
         <v>1.2904624277456649</v>
       </c>
-      <c r="P18" s="590"/>
-      <c r="Q18" s="591"/>
-      <c r="R18" s="591"/>
-      <c r="S18" s="592"/>
+      <c r="P18" s="593"/>
+      <c r="Q18" s="594"/>
+      <c r="R18" s="594"/>
+      <c r="S18" s="595"/>
       <c r="T18" s="153" t="s">
         <v>89</v>
       </c>
@@ -51278,12 +51301,12 @@
       <c r="M19" s="107"/>
       <c r="N19" s="56"/>
       <c r="O19" s="107"/>
-      <c r="P19" s="593" t="s">
+      <c r="P19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="Q19" s="594"/>
-      <c r="R19" s="594"/>
-      <c r="S19" s="595"/>
+      <c r="Q19" s="597"/>
+      <c r="R19" s="597"/>
+      <c r="S19" s="598"/>
       <c r="T19" s="161"/>
       <c r="U19" s="117"/>
       <c r="V19" s="162"/>
@@ -51317,10 +51340,10 @@
       <c r="M20" s="107"/>
       <c r="N20" s="24"/>
       <c r="O20" s="107"/>
-      <c r="P20" s="596"/>
-      <c r="Q20" s="597"/>
-      <c r="R20" s="597"/>
-      <c r="S20" s="598"/>
+      <c r="P20" s="599"/>
+      <c r="Q20" s="600"/>
+      <c r="R20" s="600"/>
+      <c r="S20" s="601"/>
       <c r="T20" s="161"/>
       <c r="U20" s="117"/>
       <c r="V20" s="162"/>
@@ -51380,11 +51403,11 @@
       <c r="N22" s="24"/>
       <c r="O22" s="20"/>
       <c r="P22" s="168"/>
-      <c r="Q22" s="599" t="s">
+      <c r="Q22" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="R22" s="599"/>
-      <c r="S22" s="600"/>
+      <c r="R22" s="602"/>
+      <c r="S22" s="603"/>
       <c r="T22" s="161"/>
       <c r="U22" s="117"/>
       <c r="V22" s="162"/>
@@ -51411,10 +51434,10 @@
       <c r="M23" s="175"/>
       <c r="N23" s="176"/>
       <c r="O23" s="177"/>
-      <c r="P23" s="601"/>
-      <c r="Q23" s="602"/>
-      <c r="R23" s="602"/>
-      <c r="S23" s="603"/>
+      <c r="P23" s="604"/>
+      <c r="Q23" s="605"/>
+      <c r="R23" s="605"/>
+      <c r="S23" s="606"/>
       <c r="T23" s="110"/>
       <c r="U23" s="178"/>
       <c r="V23" s="179"/>
@@ -51444,10 +51467,10 @@
       <c r="M24" s="187"/>
       <c r="N24" s="159"/>
       <c r="O24" s="177"/>
-      <c r="P24" s="604"/>
-      <c r="Q24" s="605"/>
-      <c r="R24" s="605"/>
-      <c r="S24" s="606"/>
+      <c r="P24" s="607"/>
+      <c r="Q24" s="608"/>
+      <c r="R24" s="608"/>
+      <c r="S24" s="609"/>
       <c r="T24" s="110"/>
       <c r="U24" s="178"/>
       <c r="V24" s="179"/>
@@ -52097,10 +52120,10 @@
       <c r="Q41" s="288"/>
       <c r="R41" s="301"/>
       <c r="S41" s="301"/>
-      <c r="T41" s="577"/>
-      <c r="U41" s="578"/>
-      <c r="V41" s="578"/>
-      <c r="W41" s="579"/>
+      <c r="T41" s="580"/>
+      <c r="U41" s="581"/>
+      <c r="V41" s="581"/>
+      <c r="W41" s="582"/>
       <c r="X41" s="302"/>
       <c r="Y41" s="303"/>
     </row>
@@ -52129,10 +52152,10 @@
       <c r="Q42" s="115"/>
       <c r="R42" s="301"/>
       <c r="S42" s="301"/>
-      <c r="T42" s="580"/>
-      <c r="U42" s="581"/>
-      <c r="V42" s="581"/>
-      <c r="W42" s="582"/>
+      <c r="T42" s="583"/>
+      <c r="U42" s="584"/>
+      <c r="V42" s="584"/>
+      <c r="W42" s="585"/>
       <c r="X42" s="302"/>
       <c r="Y42" s="303"/>
     </row>
@@ -53404,12 +53427,12 @@
         <v>16</v>
       </c>
       <c r="O3" s="20"/>
-      <c r="P3" s="583" t="s">
+      <c r="P3" s="586" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="584"/>
-      <c r="R3" s="584"/>
-      <c r="S3" s="585"/>
+      <c r="Q3" s="587"/>
+      <c r="R3" s="587"/>
+      <c r="S3" s="588"/>
       <c r="T3" s="27" t="s">
         <v>18</v>
       </c>
@@ -54070,12 +54093,12 @@
       <c r="O17" s="142">
         <v>0.4</v>
       </c>
-      <c r="P17" s="586" t="s">
+      <c r="P17" s="589" t="s">
         <v>195</v>
       </c>
-      <c r="Q17" s="587"/>
-      <c r="R17" s="588"/>
-      <c r="S17" s="589"/>
+      <c r="Q17" s="590"/>
+      <c r="R17" s="591"/>
+      <c r="S17" s="592"/>
       <c r="T17" s="143" t="s">
         <v>88</v>
       </c>
@@ -54129,10 +54152,10 @@
         <f>N18+O17</f>
         <v>1.2904624277456649</v>
       </c>
-      <c r="P18" s="590"/>
-      <c r="Q18" s="591"/>
-      <c r="R18" s="591"/>
-      <c r="S18" s="592"/>
+      <c r="P18" s="593"/>
+      <c r="Q18" s="594"/>
+      <c r="R18" s="594"/>
+      <c r="S18" s="595"/>
       <c r="T18" s="153" t="s">
         <v>89</v>
       </c>
@@ -54162,12 +54185,12 @@
       <c r="M19" s="107"/>
       <c r="N19" s="56"/>
       <c r="O19" s="107"/>
-      <c r="P19" s="593" t="s">
+      <c r="P19" s="596" t="s">
         <v>90</v>
       </c>
-      <c r="Q19" s="594"/>
-      <c r="R19" s="594"/>
-      <c r="S19" s="595"/>
+      <c r="Q19" s="597"/>
+      <c r="R19" s="597"/>
+      <c r="S19" s="598"/>
       <c r="T19" s="161"/>
       <c r="U19" s="117"/>
       <c r="V19" s="162"/>
@@ -54201,10 +54224,10 @@
       <c r="M20" s="107"/>
       <c r="N20" s="24"/>
       <c r="O20" s="107"/>
-      <c r="P20" s="596"/>
-      <c r="Q20" s="597"/>
-      <c r="R20" s="597"/>
-      <c r="S20" s="598"/>
+      <c r="P20" s="599"/>
+      <c r="Q20" s="600"/>
+      <c r="R20" s="600"/>
+      <c r="S20" s="601"/>
       <c r="T20" s="161"/>
       <c r="U20" s="117"/>
       <c r="V20" s="162"/>
@@ -54264,11 +54287,11 @@
       <c r="N22" s="24"/>
       <c r="O22" s="20"/>
       <c r="P22" s="168"/>
-      <c r="Q22" s="599" t="s">
+      <c r="Q22" s="602" t="s">
         <v>93</v>
       </c>
-      <c r="R22" s="599"/>
-      <c r="S22" s="600"/>
+      <c r="R22" s="602"/>
+      <c r="S22" s="603"/>
       <c r="T22" s="161"/>
       <c r="U22" s="117"/>
       <c r="V22" s="162"/>
@@ -54295,10 +54318,10 @@
       <c r="M23" s="175"/>
       <c r="N23" s="176"/>
       <c r="O23" s="177"/>
-      <c r="P23" s="601"/>
-      <c r="Q23" s="602"/>
-      <c r="R23" s="602"/>
-      <c r="S23" s="603"/>
+      <c r="P23" s="604"/>
+      <c r="Q23" s="605"/>
+      <c r="R23" s="605"/>
+      <c r="S23" s="606"/>
       <c r="T23" s="110"/>
       <c r="U23" s="178"/>
       <c r="V23" s="179"/>
@@ -54328,10 +54351,10 @@
       <c r="M24" s="187"/>
       <c r="N24" s="159"/>
       <c r="O24" s="177"/>
-      <c r="P24" s="604"/>
-      <c r="Q24" s="605"/>
-      <c r="R24" s="605"/>
-      <c r="S24" s="606"/>
+      <c r="P24" s="607"/>
+      <c r="Q24" s="608"/>
+      <c r="R24" s="608"/>
+      <c r="S24" s="609"/>
       <c r="T24" s="110"/>
       <c r="U24" s="178"/>
       <c r="V24" s="179"/>
@@ -54981,10 +55004,10 @@
       <c r="Q41" s="288"/>
       <c r="R41" s="301"/>
       <c r="S41" s="301"/>
-      <c r="T41" s="577"/>
-      <c r="U41" s="578"/>
-      <c r="V41" s="578"/>
-      <c r="W41" s="579"/>
+      <c r="T41" s="580"/>
+      <c r="U41" s="581"/>
+      <c r="V41" s="581"/>
+      <c r="W41" s="582"/>
       <c r="X41" s="302"/>
       <c r="Y41" s="303"/>
     </row>
@@ -55013,10 +55036,10 @@
       <c r="Q42" s="115"/>
       <c r="R42" s="301"/>
       <c r="S42" s="301"/>
-      <c r="T42" s="580"/>
-      <c r="U42" s="581"/>
-      <c r="V42" s="581"/>
-      <c r="W42" s="582"/>
+      <c r="T42" s="583"/>
+      <c r="U42" s="584"/>
+      <c r="V42" s="584"/>
+      <c r="W42" s="585"/>
       <c r="X42" s="302"/>
       <c r="Y42" s="303"/>
     </row>

</xml_diff>